<commit_message>
Extra, Allergen and interconnection done
</commit_message>
<xml_diff>
--- a/populate/data.xlsx
+++ b/populate/data.xlsx
@@ -706,10 +706,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,16 +1022,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49" style="4" customWidth="1"/>
+    <col min="4" max="4" width="81.5703125" customWidth="1"/>
     <col min="5" max="5" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
@@ -1042,7 +1048,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1070,14 +1076,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
@@ -1102,14 +1108,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
@@ -1134,14 +1140,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>215</v>
       </c>
       <c r="D4" t="s">
@@ -1169,14 +1175,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F5" t="s">
@@ -1198,14 +1204,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D6" t="s">
@@ -1230,14 +1236,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
@@ -1262,14 +1268,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D8" t="s">
@@ -1294,14 +1300,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D9" t="s">
@@ -1326,14 +1332,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D10" t="s">
@@ -1358,11 +1364,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D11" t="s">
@@ -1387,14 +1393,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
       <c r="B12" t="s">
         <v>73</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F12" t="s">
@@ -1416,14 +1422,14 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>79</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>80</v>
       </c>
       <c r="F13" t="s">
@@ -1445,11 +1451,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>81</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>216</v>
       </c>
       <c r="D14" t="s">
@@ -1474,11 +1480,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>86</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D15" t="s">
@@ -1526,14 +1532,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>95</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>96</v>
       </c>
       <c r="F17" t="s">
@@ -1555,14 +1561,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>102</v>
       </c>
       <c r="B18" t="s">
         <v>103</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D18" t="s">
@@ -1659,14 +1665,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>114</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>115</v>
       </c>
       <c r="D22" t="s">
@@ -1691,14 +1697,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>117</v>
       </c>
       <c r="B23" t="s">
         <v>118</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F23" t="s">
@@ -1720,11 +1726,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>121</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D24" t="s">
@@ -1749,14 +1755,14 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>127</v>
       </c>
       <c r="B25" t="s">
         <v>128</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>129</v>
       </c>
       <c r="F25" t="s">
@@ -1778,14 +1784,14 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>133</v>
       </c>
       <c r="B26" t="s">
         <v>128</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="4" t="s">
         <v>134</v>
       </c>
       <c r="F26" t="s">
@@ -1879,11 +1885,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>145</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D30" t="s">
@@ -1908,11 +1914,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>149</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>150</v>
       </c>
       <c r="F31" s="1">
@@ -1957,14 +1963,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>156</v>
       </c>
       <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>157</v>
       </c>
       <c r="D33" t="s">
@@ -2104,14 +2110,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>171</v>
       </c>
       <c r="B39" t="s">
         <v>95</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="4" t="s">
         <v>172</v>
       </c>
       <c r="F39" t="s">
@@ -2242,11 +2248,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>186</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="4" t="s">
         <v>187</v>
       </c>
       <c r="D45" t="s">
@@ -2274,14 +2280,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>191</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="4" t="s">
         <v>192</v>
       </c>
       <c r="D46" t="s">
@@ -2306,14 +2312,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>196</v>
       </c>
       <c r="B47" t="s">
         <v>197</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="4" t="s">
         <v>198</v>
       </c>
       <c r="F47" t="s">
@@ -2335,11 +2341,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>201</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="4" t="s">
         <v>202</v>
       </c>
       <c r="E48" t="s">
@@ -2372,11 +2378,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>208</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="4" t="s">
         <v>209</v>
       </c>
       <c r="D50" t="s">
@@ -2390,7 +2396,7 @@
       <c r="A51" t="s">
         <v>211</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="4" t="s">
         <v>212</v>
       </c>
       <c r="D51" t="s">

</xml_diff>